<commit_message>
added designer metadata fields
</commit_message>
<xml_diff>
--- a/_data/TDPS_CBMetadata.xlsx
+++ b/_data/TDPS_CBMetadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/BestChlo2016/Documents/GitHub/TDPS-Archive-CBTEST/_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4872A76A-B6E1-4245-AC62-5C726AB381AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{55480EA9-C7B5-3C46-9D57-66AFE270FA97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="680" yWindow="740" windowWidth="28040" windowHeight="17260" xr2:uid="{CB7AA178-4D61-8143-8C53-8610E077E2CF}"/>
   </bookViews>
@@ -600,7 +600,7 @@
   <dimension ref="A1:V16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q22" sqref="Q22"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1194,7 +1194,6 @@
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
@@ -1213,5 +1212,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>